<commit_message>
Configured to work with sensitivity as well as accuracy as a metric for performance
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,12 +452,147 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>a03t0000001i5dGAAQ</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Initiate the deployment of data hosting, system interface development and deployment transition activities at the VISN 20 Initial Operating Capability (IOC) sites to track for Go-Live (Q2 FY2020): Mann-Grandstaff VAMC (Spokane, WA); VA Puget Sound (Seattle/Tacoma WA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>a5Vt000000006KpEAI</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Getting our veterans through this pandemic</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>a5Vt000000006KuEAI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Helping our veterans build civilian lives of opportunity with the education and jobs worthy of their skills and talents</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>a5Vt000000006KzEAI</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ensuring that the VA welcomes all our veterans, including women veterans, veterans of color and LGBTQ veterans</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>a5Vt000000006L4EAI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Working to eliminate veteran homelessness and reducing suicide</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>a5Vt000000006L9EAI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Keeping faith with our families and caregivers</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>a5Vt000000006cyEAA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>VA operates one of the largest health care systems in the nation, providing services to more than 9 million veterans who tend to have greater health care needs than the general population. Due to challenges we identified with VA’s ability to provide timely, cost-effective, and quality care, VA health care was added to the High-Risk List in 2015 with five areas of concern: (1) ambiguous policies and inconsistent processes; (2) inadequate oversight and accountability; (3) information technology challenges; (4) inadequate training for VA staff; and (5) unclear resource needs and allocation priorities._x000D_
+_x000D_
+Since our March 2019 High-Risk Report, there are continuing concerns about VA’s ability to ensure the safety and protection of patients and staff, as well as to oversee its programs. VA’s management of its ongoing COVID-19 response underscores the significance of our concerns. For example, in February 2020 we reported on the challenges VA faces due to the increasing long-term care needs of veterans. We have identified problems with VA’s efficient use of funds, concerns amplified by VA’s estimate that its community care obligations will increase 45 percent from fiscal year 2018 to 2022 to total $21.3 billion. Additionally, VA has undertaken a number of major modernization initiatives, which were partly intended to address our high-risk concerns. As of September 2020, VA faces delays in_x000D_
+implementing these efforts, such as its new electronic health record and key financial management systems._x000D_
+_x000D_
+Since our 2019 High-Risk Report, the rating for the capacity criterion improved from not met to partially met, and ratings for the other four criteria remain unchanged. _x000D_
+ _x000D_
+As the new VA leadership team sets its priorities, it is critical that a senior leader with sufficient positional authority to drive organizational action is charged with addressing high-risk concerns._x000D_
+_x000D_
+This is particularly important as VA has made limited progress since 2015 in fully developing an action plan, although significant resources and time have been devoted to developing one._x000D_
+_x000D_
+The action plan VA approved in October 2020 included key components for most areas of concern; however, we identified deficiencies with these components. The action plan also lacked thorough integration with VA’s modernization initiatives.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>a5Vt000000006dhEAA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>The Veterans Health Administration serves upwards of 9 million veterans and is responsible for their whole health, physical and mental. Studies have found that health outcomes at VA hospitals are often better than their non-VA counterpart, and more than 90 percent of those who receive their health services through the VA report that they would recommend it to a fellow veteran. As president, Joe Biden will work to ensure that the VA provides the world class health care that our veterans have earned and deserve and sets the example for private sector care. _x000D_
+_x000D_
+In the area of mental health, the VA and DoD have done pioneering work to address the specific needs of veterans, deploying innovative treatment solutions such as telehealth and other platforms to address a variety of conditions. The private sector trails the VA in its ability to provide behavioral health services to the nation as a whole, much less to understand the unique needs of veterans. _x000D_
+_x000D_
+At the same time, the VA is also struggling with a rapidly deteriorating infrastructure, and many VA facilities are more than 60 years old. Further, across the system, the variance in quality of — and access to — care is unacceptable. As the demand for treatment has increased, the VA must continually strive to improve services and outcomes for veterans, especially in the areas of pain, polytrauma recovery, substance-use disorder (SUD), post-traumatic stress disorder (PTSD), traumatic brain injury (TBI), and general behavioral health, in the most effective and cost-efficient way possible.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>a5Vt0000000Kyu4EAC</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>VA will measure and improve Veteran Experience with VA.gov using the government-wide drivers identified for measuring customer experience (CX) with the Federal Government. By September 30, 2021, Veterans Experience scores related to VA.gov will be at least 90%, compared to a FY2020 baseline.  OMB Circ. A-11, Section 280 identifies the government-wide drivers for measuring customer experience</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reformatted parsers for bug fixes and added a tfidf tag to use_model
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,12 +452,13 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a03t0000001i5dGAAQ</t>
+          <t>001t0000009wAyPAAU</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Initiate the deployment of data hosting, system interface development and deployment transition activities at the VISN 20 Initial Operating Capability (IOC) sites to track for Go-Live (Q2 FY2020): Mann-Grandstaff VAMC (Spokane, WA); VA Puget Sound (Seattle/Tacoma WA)</t>
+          <t>The Office of the Deputy Under Secretary for Health for Operations and Management (DUSHOM/10N) leads VHA operations and ensures it continues to be the benchmark for health care excellence and value through the clinical and administrative services we provide to care for Veterans and their families._x000D_
+The Office of the DUSHOM operates VHA health care systems, medical centers, and outpatient sites of care.  VHA’s coverage area is divided into 18 Veterans Integrated Service Networks (VISN), each a shared system of care working together to better meet local health care needs and provide Veterans greater access to care.  The DUSHOM is responsible for 24 other VHA clinical and administrative program offices that ensure that VHA program policies and regulations are executed and supported to fulfill the operating needs of VHA field operations.</t>
         </is>
       </c>
     </row>
@@ -467,12 +468,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a5Vt000000006KpEAI</t>
+          <t>001t0000009wAyaAAE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Getting our veterans through this pandemic</t>
+          <t>Specialty Care Services (SCS/10P4D) is a large service, encompassing 16 distinct medical specialties, chaplaincy, nutrition and food services, as well as neurology centers of excellence and a SCS center for innovation.  SCS ensures the best overall clinical, preventive, spiritual, religious, and nutritional care is available to Veterans.  Both policy and program development utilize innovative approaches, technologies and interdisciplinary collaboration both within and outside of VHA promoting dignity and respect for our Veterans._x000D_
+SCS provides national leadership on programs and initiatives, policy matters and issues relating to care delivery, assessment of services, and outcome analysis for twenty (20) key specialty care areas._x000D_
+The Chief Consultant, in collaboration with Field-based National Program Directors, serves as the principal advisor to the Assistant Deputy Under Secretary for Health for Patient Care Services, Deputy Under Secretary for Health for Policy and Services, Principal Deputy Under Secretary for Health and Under Secretary for Health.</t>
         </is>
       </c>
     </row>
@@ -482,12 +485,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a5Vt000000006KuEAI</t>
+          <t>001t0000009wAykAAE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Helping our veterans build civilian lives of opportunity with the education and jobs worthy of their skills and talents</t>
+          <t>Patient Care Services (PCS/10P4) provides leadership for policy and program development to enable VA to provide the best possible healthcare for our Nations’ Veterans.  PCS is dedicated to ensuring the full continuum of health care, which comprises health promotion, disease prevention, diagnostics, therapeutic and rehabilitative care, recovery and palliative care.  Utilizing innovative approaches and technologies through interdisciplinary collaboration both within and outside of VHA, PCS policy and program development supports dignity and respectful care for Veterans.  Recently, the Office of Public Health realigned with PCS expanding the mission to include post-deployment health, population health, employee health and wellness, as well as a few clinical public health programs.</t>
         </is>
       </c>
     </row>
@@ -497,12 +500,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a5Vt000000006KzEAI</t>
+          <t>a03t0000001i5dGAAQ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ensuring that the VA welcomes all our veterans, including women veterans, veterans of color and LGBTQ veterans</t>
+          <t>Initiate the deployment of data hosting, system interface development and deployment transition activities at the VISN 20 Initial Operating Capability (IOC) sites to track for Go-Live (Q2 FY2020): Mann-Grandstaff VAMC (Spokane, WA); VA Puget Sound (Seattle/Tacoma WA)</t>
         </is>
       </c>
     </row>
@@ -512,87 +515,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a5Vt000000006L4EAI</t>
+          <t>a7Kt0000000KyvxEAC</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Working to eliminate veteran homelessness and reducing suicide</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>a5Vt000000006L9EAI</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Keeping faith with our families and caregivers</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>a5Vt000000006cyEAA</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>VA operates one of the largest health care systems in the nation, providing services to more than 9 million veterans who tend to have greater health care needs than the general population. Due to challenges we identified with VA’s ability to provide timely, cost-effective, and quality care, VA health care was added to the High-Risk List in 2015 with five areas of concern: (1) ambiguous policies and inconsistent processes; (2) inadequate oversight and accountability; (3) information technology challenges; (4) inadequate training for VA staff; and (5) unclear resource needs and allocation priorities._x000D_
-_x000D_
-Since our March 2019 High-Risk Report, there are continuing concerns about VA’s ability to ensure the safety and protection of patients and staff, as well as to oversee its programs. VA’s management of its ongoing COVID-19 response underscores the significance of our concerns. For example, in February 2020 we reported on the challenges VA faces due to the increasing long-term care needs of veterans. We have identified problems with VA’s efficient use of funds, concerns amplified by VA’s estimate that its community care obligations will increase 45 percent from fiscal year 2018 to 2022 to total $21.3 billion. Additionally, VA has undertaken a number of major modernization initiatives, which were partly intended to address our high-risk concerns. As of September 2020, VA faces delays in_x000D_
-implementing these efforts, such as its new electronic health record and key financial management systems._x000D_
-_x000D_
-Since our 2019 High-Risk Report, the rating for the capacity criterion improved from not met to partially met, and ratings for the other four criteria remain unchanged. _x000D_
- _x000D_
-As the new VA leadership team sets its priorities, it is critical that a senior leader with sufficient positional authority to drive organizational action is charged with addressing high-risk concerns._x000D_
-_x000D_
-This is particularly important as VA has made limited progress since 2015 in fully developing an action plan, although significant resources and time have been devoted to developing one._x000D_
-_x000D_
-The action plan VA approved in October 2020 included key components for most areas of concern; however, we identified deficiencies with these components. The action plan also lacked thorough integration with VA’s modernization initiatives.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>a5Vt000000006dhEAA</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>The Veterans Health Administration serves upwards of 9 million veterans and is responsible for their whole health, physical and mental. Studies have found that health outcomes at VA hospitals are often better than their non-VA counterpart, and more than 90 percent of those who receive their health services through the VA report that they would recommend it to a fellow veteran. As president, Joe Biden will work to ensure that the VA provides the world class health care that our veterans have earned and deserve and sets the example for private sector care. _x000D_
-_x000D_
-In the area of mental health, the VA and DoD have done pioneering work to address the specific needs of veterans, deploying innovative treatment solutions such as telehealth and other platforms to address a variety of conditions. The private sector trails the VA in its ability to provide behavioral health services to the nation as a whole, much less to understand the unique needs of veterans. _x000D_
-_x000D_
-At the same time, the VA is also struggling with a rapidly deteriorating infrastructure, and many VA facilities are more than 60 years old. Further, across the system, the variance in quality of — and access to — care is unacceptable. As the demand for treatment has increased, the VA must continually strive to improve services and outcomes for veterans, especially in the areas of pain, polytrauma recovery, substance-use disorder (SUD), post-traumatic stress disorder (PTSD), traumatic brain injury (TBI), and general behavioral health, in the most effective and cost-efficient way possible.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>a5Vt0000000Kyu4EAC</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>VA will measure and improve Veteran Experience with VA.gov using the government-wide drivers identified for measuring customer experience (CX) with the Federal Government. By September 30, 2021, Veterans Experience scores related to VA.gov will be at least 90%, compared to a FY2020 baseline.  OMB Circ. A-11, Section 280 identifies the government-wide drivers for measuring customer experience</t>
+          <t>Functions of Veterans Health Administration: in general</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to now run model on multiple component descriptions at once
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,37 +1,101 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+  <si>
+    <t>Related Component</t>
+  </si>
+  <si>
+    <t>Related Component ID</t>
+  </si>
+  <si>
+    <t>Related Component Description</t>
+  </si>
+  <si>
+    <t>VHA-15 Operations</t>
+  </si>
+  <si>
+    <t>VHA-11SPEC Specialty Care</t>
+  </si>
+  <si>
+    <t>VHA-12 Patient Care Services</t>
+  </si>
+  <si>
+    <t>Electronic Health Records Modernization (EHRM)</t>
+  </si>
+  <si>
+    <t>Functions of Veterans Health Administration: in general</t>
+  </si>
+  <si>
+    <t>001t0000009wAyPAAU</t>
+  </si>
+  <si>
+    <t>001t0000009wAyaAAE</t>
+  </si>
+  <si>
+    <t>001t0000009wAykAAE</t>
+  </si>
+  <si>
+    <t>a03t0000001i5dGAAQ</t>
+  </si>
+  <si>
+    <t>a7Kt0000000KyvxEAC</t>
+  </si>
+  <si>
+    <t>The Office of the Deputy Under Secretary for Health for Operations and Management (DUSHOM/10N) leads VHA operations and ensures it continues to be the benchmark for health care excellence and value through the clinical and administrative services we provide to care for Veterans and their families._x005F_x000D_
+The Office of the DUSHOM operates VHA health care systems, medical centers, and outpatient sites of care.  VHA’s coverage area is divided into 18 Veterans Integrated Service Networks (VISN), each a shared system of care working together to better meet local health care needs and provide Veterans greater access to care.  The DUSHOM is responsible for 24 other VHA clinical and administrative program offices that ensure that VHA program policies and regulations are executed and supported to fulfill the operating needs of VHA field operations.</t>
+  </si>
+  <si>
+    <t>Specialty Care Services (SCS/10P4D) is a large service, encompassing 16 distinct medical specialties, chaplaincy, nutrition and food services, as well as neurology centers of excellence and a SCS center for innovation.  SCS ensures the best overall clinical, preventive, spiritual, religious, and nutritional care is available to Veterans.  Both policy and program development utilize innovative approaches, technologies and interdisciplinary collaboration both within and outside of VHA promoting dignity and respect for our Veterans._x005F_x000D_
+SCS provides national leadership on programs and initiatives, policy matters and issues relating to care delivery, assessment of services, and outcome analysis for twenty (20) key specialty care areas._x005F_x000D_
+The Chief Consultant, in collaboration with Field-based National Program Directors, serves as the principal advisor to the Assistant Deputy Under Secretary for Health for Patient Care Services, Deputy Under Secretary for Health for Policy and Services, Principal Deputy Under Secretary for Health and Under Secretary for Health.</t>
+  </si>
+  <si>
+    <t>Patient Care Services (PCS/10P4) provides leadership for policy and program development to enable VA to provide the best possible healthcare for our Nations’ Veterans.  PCS is dedicated to ensuring the full continuum of health care, which comprises health promotion, disease prevention, diagnostics, therapeutic and rehabilitative care, recovery and palliative care.  Utilizing innovative approaches and technologies through interdisciplinary collaboration both within and outside of VHA, PCS policy and program development supports dignity and respectful care for Veterans.  Recently, the Office of Public Health realigned with PCS expanding the mission to include post-deployment health, population health, employee health and wellness, as well as a few clinical public health programs.</t>
+  </si>
+  <si>
+    <t>Initiate the deployment of data hosting, system interface development and deployment transition activities at the VISN 20 Initial Operating Capability (IOC) sites to track for Go-Live (Q2 FY2020): Mann-Grandstaff VAMC (Spokane, WA); VA Puget Sound (Seattle/Tacoma WA)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +110,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -421,110 +426,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="1080.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Related Component ID</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Related Component Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>001t0000009wAyPAAU</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The Office of the Deputy Under Secretary for Health for Operations and Management (DUSHOM/10N) leads VHA operations and ensures it continues to be the benchmark for health care excellence and value through the clinical and administrative services we provide to care for Veterans and their families._x000D_
-The Office of the DUSHOM operates VHA health care systems, medical centers, and outpatient sites of care.  VHA’s coverage area is divided into 18 Veterans Integrated Service Networks (VISN), each a shared system of care working together to better meet local health care needs and provide Veterans greater access to care.  The DUSHOM is responsible for 24 other VHA clinical and administrative program offices that ensure that VHA program policies and regulations are executed and supported to fulfill the operating needs of VHA field operations.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>001t0000009wAyaAAE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Specialty Care Services (SCS/10P4D) is a large service, encompassing 16 distinct medical specialties, chaplaincy, nutrition and food services, as well as neurology centers of excellence and a SCS center for innovation.  SCS ensures the best overall clinical, preventive, spiritual, religious, and nutritional care is available to Veterans.  Both policy and program development utilize innovative approaches, technologies and interdisciplinary collaboration both within and outside of VHA promoting dignity and respect for our Veterans._x000D_
-SCS provides national leadership on programs and initiatives, policy matters and issues relating to care delivery, assessment of services, and outcome analysis for twenty (20) key specialty care areas._x000D_
-The Chief Consultant, in collaboration with Field-based National Program Directors, serves as the principal advisor to the Assistant Deputy Under Secretary for Health for Patient Care Services, Deputy Under Secretary for Health for Policy and Services, Principal Deputy Under Secretary for Health and Under Secretary for Health.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>001t0000009wAykAAE</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Patient Care Services (PCS/10P4) provides leadership for policy and program development to enable VA to provide the best possible healthcare for our Nations’ Veterans.  PCS is dedicated to ensuring the full continuum of health care, which comprises health promotion, disease prevention, diagnostics, therapeutic and rehabilitative care, recovery and palliative care.  Utilizing innovative approaches and technologies through interdisciplinary collaboration both within and outside of VHA, PCS policy and program development supports dignity and respectful care for Veterans.  Recently, the Office of Public Health realigned with PCS expanding the mission to include post-deployment health, population health, employee health and wellness, as well as a few clinical public health programs.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>a03t0000001i5dGAAQ</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Initiate the deployment of data hosting, system interface development and deployment transition activities at the VISN 20 Initial Operating Capability (IOC) sites to track for Go-Live (Q2 FY2020): Mann-Grandstaff VAMC (Spokane, WA); VA Puget Sound (Seattle/Tacoma WA)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>a7Kt0000000KyvxEAC</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Functions of Veterans Health Administration: in general</t>
-        </is>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="nan" customWidth="1"/>
+    <col min="2" max="2" width="nan" customWidth="1"/>
+    <col min="3" max="3" width="nan" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="267.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up environment and removed rapids as it is currently unused
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -432,11 +432,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="55.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="1080.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
@@ -531,11 +526,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="nan" customWidth="1"/>
-    <col min="2" max="2" width="nan" customWidth="1"/>
-    <col min="3" max="3" width="nan" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
@@ -560,11 +550,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="46.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="267.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">

</xml_diff>